<commit_message>
fix: Change to pivot table structure for quartile SQL data
</commit_message>
<xml_diff>
--- a/csv-files/family-cat-quartiles.xlsx
+++ b/csv-files/family-cat-quartiles.xlsx
@@ -7,15 +7,19 @@
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart3" sheetId="4" r:id="rId1"/>
-    <sheet name="family-cat-quartiles" sheetId="1" r:id="rId2"/>
+    <sheet name="family-quartiles-stackedbar" sheetId="6" r:id="rId1"/>
+    <sheet name="pt-family-cat-quartiles" sheetId="5" r:id="rId2"/>
+    <sheet name="family-cat-quartiles" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId4"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="17">
   <si>
     <t>category</t>
   </si>
@@ -54,6 +58,18 @@
   </si>
   <si>
     <t>Music</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Sum of quartile_count</t>
   </si>
 </sst>
 </file>
@@ -538,8 +554,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -602,12 +623,16 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="103"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="3"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[family-cat-quartiles.xlsx]pt-family-cat-quartiles!PivotTable1</c:name>
+    <c:fmtId val="1"/>
+  </c:pivotSource>
   <c:chart>
     <c:title>
       <c:tx>
@@ -619,14 +644,14 @@
               <a:defRPr sz="3200"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="3200"/>
+              <a:rPr lang="en-ZA" sz="3200"/>
               <a:t>Family-Friendly</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="3200" baseline="0"/>
+              <a:rPr lang="en-ZA" sz="3200" baseline="0"/>
               <a:t> Categories Quartiles</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="3200"/>
+            <a:endParaRPr lang="en-ZA" sz="3200"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -634,6 +659,56 @@
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+      </c:pivotFmt>
+    </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -645,194 +720,271 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'family-cat-quartiles'!$C$1</c:f>
+              <c:f>'pt-family-cat-quartiles'!$B$3:$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>quartile_count</c:v>
+                  <c:v>1st_quartile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'family-cat-quartiles'!$A$2:$B$25</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="24"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>1st_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>2nd_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3rd_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>4th_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1st_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>2nd_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>3rd_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>4th_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>1st_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>2nd_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>3rd_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>4th_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>1st_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>2nd_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>3rd_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>4th_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>1st_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>2nd_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>3rd_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>4th_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>1st_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>2nd_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>3rd_quartile</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>4th_quartile</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Animation</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Children</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Classics</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Comedy</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>Family</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>Music</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+            <c:strRef>
+              <c:f>'pt-family-cat-quartiles'!$A$5:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Animation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Children</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Classics</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Comedy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Family</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Music</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'family-cat-quartiles'!$C$2:$C$25</c:f>
+              <c:f>'pt-family-cat-quartiles'!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pt-family-cat-quartiles'!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2nd_quartile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'pt-family-cat-quartiles'!$A$5:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Animation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Children</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Classics</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Comedy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Family</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Music</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'pt-family-cat-quartiles'!$C$5:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pt-family-cat-quartiles'!$D$3:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3rd_quartile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'pt-family-cat-quartiles'!$A$5:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Animation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Children</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Classics</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Comedy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Family</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Music</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'pt-family-cat-quartiles'!$D$5:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pt-family-cat-quartiles'!$E$3:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4th_quartile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'pt-family-cat-quartiles'!$A$5:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Animation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Children</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Classics</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Comedy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Family</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Music</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'pt-family-cat-quartiles'!$E$5:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="23">
                   <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
@@ -841,19 +993,19 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="75"/>
+        <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="41644032"/>
-        <c:axId val="41645568"/>
+        <c:axId val="39019264"/>
+        <c:axId val="39021184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41644032"/>
+        <c:axId val="39019264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -881,7 +1033,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41645568"/>
+        <c:crossAx val="39021184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -889,12 +1041,13 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41645568"/>
+        <c:axId val="39021184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -918,15 +1071,28 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41644032"/>
+        <c:crossAx val="39019264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneSeries val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
 </c:chartSpace>
 </file>
 
@@ -966,6 +1132,457 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Raeez" refreshedDate="44355.483553356484" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="24">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:C25" sheet="family-cat-quartiles"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="category" numFmtId="0">
+      <sharedItems count="6">
+        <s v="Animation"/>
+        <s v="Children"/>
+        <s v="Classics"/>
+        <s v="Comedy"/>
+        <s v="Family"/>
+        <s v="Music"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="quartile_type" numFmtId="0">
+      <sharedItems count="4">
+        <s v="1st_quartile"/>
+        <s v="2nd_quartile"/>
+        <s v="3rd_quartile"/>
+        <s v="4th_quartile"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="quartile_count" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="10" maxValue="22"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="24">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="22"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="16"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="17"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="16"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="12"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="20"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="21"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="19"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="12"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A3:F11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of quartile_count" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="16">
+    <chartFormat chart="1" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="12" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="13" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="14" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="15" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="16" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="17" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="18" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1255,10 +1872,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3">
+        <v>15</v>
+      </c>
+      <c r="F8" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3">
+        <v>21</v>
+      </c>
+      <c r="F9" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3">
+        <v>19</v>
+      </c>
+      <c r="E10" s="3">
+        <v>12</v>
+      </c>
+      <c r="F10" s="3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3">
+        <v>87</v>
+      </c>
+      <c r="C11" s="3">
+        <v>81</v>
+      </c>
+      <c r="D11" s="3">
+        <v>98</v>
+      </c>
+      <c r="E11" s="3">
+        <v>95</v>
+      </c>
+      <c r="F11" s="3">
+        <v>361</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,6 +2096,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -1297,6 +2107,9 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -1305,6 +2118,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -1324,6 +2140,9 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -1332,6 +2151,9 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -1340,6 +2162,9 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -1359,6 +2184,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -1367,6 +2195,9 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -1375,6 +2206,9 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -1394,6 +2228,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
@@ -1402,6 +2239,9 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
@@ -1410,6 +2250,9 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -1429,6 +2272,9 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
@@ -1437,6 +2283,9 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
@@ -1445,6 +2294,9 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -1464,6 +2316,9 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
@@ -1472,6 +2327,9 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -1480,6 +2338,9 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>

</xml_diff>